<commit_message>
Dataset reorganizado Removi as músicas dos generos nao utilizados Atualizei os xlsx relacionados às musicas tambem pequenos ajustes na exibicao de progresso da criacao de espectrogramas
</commit_message>
<xml_diff>
--- a/generos.xlsx
+++ b/generos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="8">
   <si>
     <t>id</t>
   </si>
@@ -19,13 +19,7 @@
     <t>genero</t>
   </si>
   <si>
-    <t>Instrumental</t>
-  </si>
-  <si>
     <t>Rock</t>
-  </si>
-  <si>
-    <t>Soul</t>
   </si>
   <si>
     <t>Pop</t>
@@ -37,19 +31,10 @@
     <t>Classical</t>
   </si>
   <si>
-    <t>Hip hop</t>
-  </si>
-  <si>
-    <t>Folk</t>
-  </si>
-  <si>
     <t>Jazz</t>
   </si>
   <si>
     <t>Country</t>
-  </si>
-  <si>
-    <t>Blues</t>
   </si>
 </sst>
 </file>
@@ -799,7 +784,7 @@
         <v>61.0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
@@ -807,7 +792,7 @@
         <v>62.0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64">
@@ -815,7 +800,7 @@
         <v>63.0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65">
@@ -823,7 +808,7 @@
         <v>64.0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66">
@@ -831,7 +816,7 @@
         <v>65.0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
@@ -839,7 +824,7 @@
         <v>66.0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -847,7 +832,7 @@
         <v>67.0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -855,7 +840,7 @@
         <v>68.0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
@@ -863,7 +848,7 @@
         <v>69.0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -871,7 +856,7 @@
         <v>70.0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
@@ -879,7 +864,7 @@
         <v>71.0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
@@ -887,7 +872,7 @@
         <v>72.0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74">
@@ -895,7 +880,7 @@
         <v>73.0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75">
@@ -903,7 +888,7 @@
         <v>74.0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76">
@@ -911,7 +896,7 @@
         <v>75.0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
@@ -919,7 +904,7 @@
         <v>76.0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78">
@@ -927,7 +912,7 @@
         <v>77.0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79">
@@ -935,7 +920,7 @@
         <v>78.0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80">
@@ -943,7 +928,7 @@
         <v>79.0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81">
@@ -951,7 +936,7 @@
         <v>80.0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82">
@@ -959,7 +944,7 @@
         <v>81.0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83">
@@ -967,7 +952,7 @@
         <v>82.0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84">
@@ -975,7 +960,7 @@
         <v>83.0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85">
@@ -983,7 +968,7 @@
         <v>84.0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86">
@@ -991,7 +976,7 @@
         <v>85.0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
@@ -999,7 +984,7 @@
         <v>86.0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88">
@@ -1007,7 +992,7 @@
         <v>87.0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89">
@@ -1015,7 +1000,7 @@
         <v>88.0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90">
@@ -1023,7 +1008,7 @@
         <v>89.0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91">
@@ -1031,7 +1016,7 @@
         <v>90.0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92">
@@ -1039,7 +1024,7 @@
         <v>91.0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93">
@@ -1047,7 +1032,7 @@
         <v>92.0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94">
@@ -1055,7 +1040,7 @@
         <v>93.0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95">
@@ -1063,7 +1048,7 @@
         <v>94.0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96">
@@ -1071,7 +1056,7 @@
         <v>95.0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97">
@@ -1079,7 +1064,7 @@
         <v>96.0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98">
@@ -1087,7 +1072,7 @@
         <v>97.0</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99">
@@ -1095,7 +1080,7 @@
         <v>98.0</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100">
@@ -1103,7 +1088,7 @@
         <v>99.0</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101">
@@ -1111,7 +1096,7 @@
         <v>100.0</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102">
@@ -1119,7 +1104,7 @@
         <v>101.0</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103">
@@ -1127,7 +1112,7 @@
         <v>102.0</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104">
@@ -1135,7 +1120,7 @@
         <v>103.0</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105">
@@ -1143,7 +1128,7 @@
         <v>104.0</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106">
@@ -1151,7 +1136,7 @@
         <v>105.0</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107">
@@ -1159,7 +1144,7 @@
         <v>106.0</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108">
@@ -1167,7 +1152,7 @@
         <v>107.0</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109">
@@ -1175,7 +1160,7 @@
         <v>108.0</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110">
@@ -1183,7 +1168,7 @@
         <v>109.0</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111">
@@ -1191,7 +1176,7 @@
         <v>110.0</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112">
@@ -1199,7 +1184,7 @@
         <v>111.0</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113">
@@ -1207,7 +1192,7 @@
         <v>112.0</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114">
@@ -1215,7 +1200,7 @@
         <v>113.0</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115">
@@ -1223,7 +1208,7 @@
         <v>114.0</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="116">
@@ -1231,7 +1216,7 @@
         <v>115.0</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117">
@@ -1239,7 +1224,7 @@
         <v>116.0</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118">
@@ -1247,7 +1232,7 @@
         <v>117.0</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119">
@@ -1255,7 +1240,7 @@
         <v>118.0</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120">
@@ -1263,7 +1248,7 @@
         <v>119.0</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121">
@@ -1271,7 +1256,7 @@
         <v>120.0</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122">
@@ -1279,7 +1264,7 @@
         <v>121.0</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="123">
@@ -1287,7 +1272,7 @@
         <v>122.0</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124">
@@ -1295,7 +1280,7 @@
         <v>123.0</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125">
@@ -1303,7 +1288,7 @@
         <v>124.0</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126">
@@ -1311,7 +1296,7 @@
         <v>125.0</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127">
@@ -1319,7 +1304,7 @@
         <v>126.0</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128">
@@ -1327,7 +1312,7 @@
         <v>127.0</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129">
@@ -1335,7 +1320,7 @@
         <v>128.0</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130">
@@ -1343,7 +1328,7 @@
         <v>129.0</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131">
@@ -1351,7 +1336,7 @@
         <v>130.0</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132">
@@ -1359,7 +1344,7 @@
         <v>131.0</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133">
@@ -1367,7 +1352,7 @@
         <v>132.0</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134">
@@ -1375,7 +1360,7 @@
         <v>133.0</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135">
@@ -1383,7 +1368,7 @@
         <v>134.0</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136">
@@ -1391,7 +1376,7 @@
         <v>135.0</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137">
@@ -1399,7 +1384,7 @@
         <v>136.0</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138">
@@ -1407,7 +1392,7 @@
         <v>137.0</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139">
@@ -1415,7 +1400,7 @@
         <v>138.0</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140">
@@ -1423,7 +1408,7 @@
         <v>139.0</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141">
@@ -1431,7 +1416,7 @@
         <v>140.0</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142">
@@ -1439,7 +1424,7 @@
         <v>141.0</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="143">
@@ -1447,7 +1432,7 @@
         <v>142.0</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144">
@@ -1455,7 +1440,7 @@
         <v>143.0</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="145">
@@ -1463,7 +1448,7 @@
         <v>144.0</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="146">
@@ -1471,7 +1456,7 @@
         <v>145.0</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="147">
@@ -1479,7 +1464,7 @@
         <v>146.0</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="148">
@@ -1487,7 +1472,7 @@
         <v>147.0</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="149">
@@ -1495,7 +1480,7 @@
         <v>148.0</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="150">
@@ -1503,7 +1488,7 @@
         <v>149.0</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="151">
@@ -1511,7 +1496,7 @@
         <v>150.0</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="152">
@@ -1519,7 +1504,7 @@
         <v>151.0</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="153">
@@ -1527,7 +1512,7 @@
         <v>152.0</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="154">
@@ -1535,7 +1520,7 @@
         <v>153.0</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="155">
@@ -1543,7 +1528,7 @@
         <v>154.0</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="156">
@@ -1551,7 +1536,7 @@
         <v>155.0</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="157">
@@ -1559,7 +1544,7 @@
         <v>156.0</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="158">
@@ -1567,7 +1552,7 @@
         <v>157.0</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="159">
@@ -1575,7 +1560,7 @@
         <v>158.0</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="160">
@@ -1583,7 +1568,7 @@
         <v>159.0</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="161">
@@ -1591,7 +1576,7 @@
         <v>160.0</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="162">
@@ -1599,7 +1584,7 @@
         <v>161.0</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="163">
@@ -1607,7 +1592,7 @@
         <v>162.0</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="164">
@@ -1615,7 +1600,7 @@
         <v>163.0</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="165">
@@ -1623,7 +1608,7 @@
         <v>164.0</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="166">
@@ -1631,7 +1616,7 @@
         <v>165.0</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="167">
@@ -1639,7 +1624,7 @@
         <v>166.0</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="168">
@@ -1647,7 +1632,7 @@
         <v>167.0</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="169">
@@ -1655,7 +1640,7 @@
         <v>168.0</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="170">
@@ -1663,7 +1648,7 @@
         <v>169.0</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="171">
@@ -1671,7 +1656,7 @@
         <v>170.0</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="172">
@@ -1679,7 +1664,7 @@
         <v>171.0</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="173">
@@ -1687,7 +1672,7 @@
         <v>172.0</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="174">
@@ -1695,7 +1680,7 @@
         <v>173.0</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="175">
@@ -1703,7 +1688,7 @@
         <v>174.0</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="176">
@@ -1711,7 +1696,7 @@
         <v>175.0</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="177">
@@ -1719,7 +1704,7 @@
         <v>176.0</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="178">
@@ -1727,7 +1712,7 @@
         <v>177.0</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="179">
@@ -1735,7 +1720,7 @@
         <v>178.0</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="180">
@@ -1743,7 +1728,7 @@
         <v>179.0</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="181">
@@ -1751,567 +1736,7 @@
         <v>180.0</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" s="1">
-        <v>181.0</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="1">
-        <v>182.0</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" s="1">
-        <v>183.0</v>
-      </c>
-      <c r="B184" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" s="1">
-        <v>184.0</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" s="1">
-        <v>185.0</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" s="1">
-        <v>186.0</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" s="1">
-        <v>187.0</v>
-      </c>
-      <c r="B188" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" s="1">
-        <v>188.0</v>
-      </c>
-      <c r="B189" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" s="1">
-        <v>189.0</v>
-      </c>
-      <c r="B190" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" s="1">
-        <v>190.0</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" s="1">
-        <v>191.0</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" s="1">
-        <v>192.0</v>
-      </c>
-      <c r="B193" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" s="1">
-        <v>193.0</v>
-      </c>
-      <c r="B194" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" s="1">
-        <v>194.0</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" s="1">
-        <v>195.0</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" s="1">
-        <v>196.0</v>
-      </c>
-      <c r="B197" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" s="1">
-        <v>197.0</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" s="1">
-        <v>198.0</v>
-      </c>
-      <c r="B199" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" s="1">
-        <v>199.0</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" s="1">
-        <v>200.0</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" s="1">
-        <v>201.0</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" s="1">
-        <v>202.0</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" s="1">
-        <v>203.0</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" s="1">
-        <v>204.0</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" s="1">
-        <v>205.0</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" s="1">
-        <v>206.0</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" s="1">
-        <v>207.0</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" s="1">
-        <v>208.0</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" s="1">
-        <v>209.0</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" s="1">
-        <v>210.0</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" s="1">
-        <v>211.0</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" s="1">
-        <v>212.0</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" s="1">
-        <v>213.0</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" s="1">
-        <v>214.0</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" s="1">
-        <v>215.0</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" s="1">
-        <v>216.0</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" s="1">
-        <v>217.0</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" s="1">
-        <v>218.0</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" s="1">
-        <v>219.0</v>
-      </c>
-      <c r="B220" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" s="1">
-        <v>220.0</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" s="1">
-        <v>221.0</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" s="1">
-        <v>222.0</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" s="1">
-        <v>223.0</v>
-      </c>
-      <c r="B224" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" s="1">
-        <v>224.0</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" s="1">
-        <v>225.0</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" s="1">
-        <v>226.0</v>
-      </c>
-      <c r="B227" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" s="1">
-        <v>227.0</v>
-      </c>
-      <c r="B228" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" s="1">
-        <v>228.0</v>
-      </c>
-      <c r="B229" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" s="1">
-        <v>229.0</v>
-      </c>
-      <c r="B230" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" s="1">
-        <v>230.0</v>
-      </c>
-      <c r="B231" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" s="1">
-        <v>231.0</v>
-      </c>
-      <c r="B232" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" s="1">
-        <v>232.0</v>
-      </c>
-      <c r="B233" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" s="1">
-        <v>233.0</v>
-      </c>
-      <c r="B234" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" s="1">
-        <v>234.0</v>
-      </c>
-      <c r="B235" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" s="1">
-        <v>235.0</v>
-      </c>
-      <c r="B236" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" s="1">
-        <v>236.0</v>
-      </c>
-      <c r="B237" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" s="1">
-        <v>237.0</v>
-      </c>
-      <c r="B238" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" s="1">
-        <v>238.0</v>
-      </c>
-      <c r="B239" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" s="1">
-        <v>239.0</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" s="1">
-        <v>240.0</v>
-      </c>
-      <c r="B241" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" s="1">
-        <v>241.0</v>
-      </c>
-      <c r="B242" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" s="1">
-        <v>242.0</v>
-      </c>
-      <c r="B243" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" s="1">
-        <v>243.0</v>
-      </c>
-      <c r="B244" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" s="1">
-        <v>244.0</v>
-      </c>
-      <c r="B245" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" s="1">
-        <v>245.0</v>
-      </c>
-      <c r="B246" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" s="1">
-        <v>246.0</v>
-      </c>
-      <c r="B247" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" s="1">
-        <v>247.0</v>
-      </c>
-      <c r="B248" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" s="1">
-        <v>248.0</v>
-      </c>
-      <c r="B249" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" s="1">
-        <v>249.0</v>
-      </c>
-      <c r="B250" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251" s="1">
-        <v>250.0</v>
-      </c>
-      <c r="B251" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>